<commit_message>
Add new JIRA utilities and enhance existing reports
New Features:
- nh-defect-upload.js: CSV to JIRA bug import with duplicate detection
  - Maps UAT defects to JIRA bugs under Epic VER10-8245
  - Auto-assigns to Caroline Wallen, sets fixVersion to Release 1C
  - Priority mapping (P1-P4) and formatted descriptions

- generate-dev-review-by-assignee.js: Dev/Review status report
  - Shows current sprint tickets in 'In Dev' and 'In Review' by assignee
  - Groups by status first, then by assignee with story point totals
  - Case-insensitive status matching

Enhancements:
- generate-work-done-today-report.js: Added sprint totals
  - Now shows both today's activity and sprint-to-date totals
  - Includes completed issues and story points for NH Sprint 31
  - Better context for daily progress tracking

Dependencies:
- Added csv-parse for CSV file parsing

Data:
- Added CCET Release 1 C UAT Defect Log.csv for defect tracking
- Updated NH Story Point Plan.xlsx with latest sprint data
</commit_message>
<xml_diff>
--- a/data/NH Story Point Plan.xlsx
+++ b/data/NH Story Point Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="-20240" windowWidth="30240" windowHeight="18960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Full-Delivery" state="visible" r:id="rId4"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="134" zoomScaleNormal="120">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="0" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
@@ -2968,7 +2968,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="29">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2989,7 +2989,7 @@
         <v>215</v>
       </c>
       <c r="E50" s="33">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
@@ -3339,7 +3339,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -3658,7 +3658,9 @@
       <c r="F3" s="9">
         <v>18</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9">
+        <v>22</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -3851,118 +3853,118 @@
         <v>55</v>
       </c>
       <c r="G5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="H5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="I5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="J5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="K5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="L5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="M5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="N5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="O5" s="9">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="P5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="R5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="S5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="T5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="U5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="V5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="W5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="X5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Y5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Z5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AA5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AB5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AC5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AD5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AE5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AF5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AG5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AH5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AI5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AJ5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AK5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AL5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AM5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AN5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AO5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AP5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AQ5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="AR5" s="42">
-        <v>55</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
@@ -3984,7 +3986,9 @@
       <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>-8</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -4043,118 +4047,118 @@
         <v>714</v>
       </c>
       <c r="G7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="H7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="I7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="J7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="K7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="L7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="M7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="N7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="O7" s="9">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="P7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="Q7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="R7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="S7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="T7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="U7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="V7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="W7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="X7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="Y7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="Z7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AA7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AB7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AC7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AD7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AE7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AF7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AG7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AH7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AI7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AJ7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AK7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AL7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AM7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AN7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AO7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AP7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AQ7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="AR7" s="42">
-        <v>714</v>
+        <v>692</v>
       </c>
     </row>
   </sheetData>
@@ -5283,7 +5287,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -6117,20 +6121,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="47">
-        <v>15.33</v>
+        <v>17</v>
       </c>
       <c r="C24" s="47">
-        <v>15.33</v>
+        <v>17</v>
       </c>
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
       <c r="F24" s="47">
-        <v>15.33</v>
+        <v>17</v>
+      </c>
+      <c r="G24" s="47">
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -6296,7 +6303,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -7123,7 +7130,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -7915,7 +7922,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -8742,7 +8749,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -9534,7 +9541,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -10186,7 +10193,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -10523,6 +10530,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add dry-run feature to defect upload script
- Added --dry-run command-line flag for preview mode
- In dry-run mode, shows what bugs would be created without making changes
- Displays all field values: summary, priority, assignee, fix version, epic link
- Still validates CSV data, checks for duplicates, and maps priorities
- Perfect for verifying data before bulk upload
- Fixed CSV file path (added space in filename)
- Updated README with dry-run documentation and examples
- Enhanced console output to clearly distinguish dry-run vs real mode
</commit_message>
<xml_diff>
--- a/data/NH Story Point Plan.xlsx
+++ b/data/NH Story Point Plan.xlsx
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="134" zoomScaleNormal="120">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="0" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
@@ -2968,7 +2968,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="29">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2989,7 +2989,7 @@
         <v>215</v>
       </c>
       <c r="E50" s="33">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
@@ -3348,7 +3348,7 @@
   <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="150" zoomScaleNormal="125">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
@@ -3659,7 +3659,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="9">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -3853,118 +3853,118 @@
         <v>55</v>
       </c>
       <c r="G5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O5" s="9">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="S5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="U5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="V5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="W5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="X5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Y5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AA5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AB5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AC5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AD5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AE5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AF5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AG5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AH5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AI5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AJ5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AK5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AL5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AM5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AN5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AO5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AP5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AQ5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AR5" s="42">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
@@ -3987,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="9">
-        <v>-8</v>
+        <v>-11</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -4047,118 +4047,118 @@
         <v>714</v>
       </c>
       <c r="G7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="H7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="I7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="J7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="K7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="L7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="M7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="N7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="O7" s="9">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="P7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="Q7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="R7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="S7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="T7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="U7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="V7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="W7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="X7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="Y7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="Z7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AA7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AB7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AC7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AD7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AE7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AF7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AG7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AH7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AI7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AJ7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AK7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AL7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AM7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AN7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AO7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AP7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AQ7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="AR7" s="42">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -6126,18 +6126,18 @@
         <v>69</v>
       </c>
       <c r="B24" s="47">
-        <v>17</v>
+        <v>16.25</v>
       </c>
       <c r="C24" s="47">
-        <v>17</v>
+        <v>16.25</v>
       </c>
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
       <c r="F24" s="47">
-        <v>17</v>
+        <v>16.25</v>
       </c>
       <c r="G24" s="47">
-        <v>17</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>